<commit_message>
Forms to start round
</commit_message>
<xml_diff>
--- a/xls/COST_PCD.xlsx
+++ b/xls/COST_PCD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12735"/>
+    <workbookView windowWidth="24300" windowHeight="13695"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120">
   <si>
     <t>type</t>
   </si>
@@ -99,13 +99,13 @@
     <t>Código do Centro de Saúde</t>
   </si>
   <si>
-    <t>formato XXXX</t>
+    <t>formato 0XX</t>
   </si>
   <si>
-    <t>regex(., '^[0-9][0-9][0-9][0-9]$')</t>
+    <t>regex(., '^[0][0-9][0-9]$')</t>
   </si>
   <si>
-    <t>Apenas 4 digitos</t>
+    <t>Apenas 3 digitos iniciando com zero</t>
   </si>
   <si>
     <t>yes</t>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Código do trabalhador sanitário</t>
+  </si>
+  <si>
+    <t>formato XXX</t>
+  </si>
+  <si>
+    <t>regex(., '^[0-9][0-9][0-9]$')</t>
+  </si>
+  <si>
+    <t>Apenas 3 digitos</t>
   </si>
   <si>
     <t>date</t>
@@ -129,12 +138,6 @@
     <t>.&lt;=today()</t>
   </si>
   <si>
-    <t>study</t>
-  </si>
-  <si>
-    <t>Estudo ID</t>
-  </si>
-  <si>
     <t>select_one gender</t>
   </si>
   <si>
@@ -144,16 +147,28 @@
     <t>Sexo</t>
   </si>
   <si>
+    <t>integer</t>
+  </si>
+  <si>
     <t>locality</t>
   </si>
   <si>
     <t>Localidade</t>
   </si>
   <si>
-    <t>neighborhood</t>
+    <t>village</t>
   </si>
   <si>
     <t>Bairro</t>
+  </si>
+  <si>
+    <t>Formato 7XXX</t>
+  </si>
+  <si>
+    <t>regex(., '^[7][0-9][0-9][0-9]$')</t>
+  </si>
+  <si>
+    <t>Apenas 4 digitos iniciando com sete</t>
   </si>
   <si>
     <t>select_one ages</t>
@@ -234,13 +249,22 @@
     <t>Data de Admissão</t>
   </si>
   <si>
+    <t>A data de admissão deve menor ou igual a data de hoje</t>
+  </si>
+  <si>
+    <t>${source} = 2</t>
+  </si>
+  <si>
     <t>discharge_date</t>
   </si>
   <si>
     <t>Data de alta</t>
   </si>
   <si>
-    <t>.&gt;=${intern_date}</t>
+    <t>.&gt;=${intern_date} and .&lt;=today()</t>
+  </si>
+  <si>
+    <t>A data de alta deve ser maior que data de admissão e menor ou igual a data de hoje</t>
   </si>
   <si>
     <t>select_one outcomes</t>
@@ -250,9 +274,6 @@
   </si>
   <si>
     <t>Resultado</t>
-  </si>
-  <si>
-    <t>integer</t>
   </si>
   <si>
     <t>processed</t>
@@ -397,11 +418,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,7 +447,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -434,6 +469,52 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -448,44 +529,6 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -505,37 +548,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -543,15 +557,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -572,6 +578,28 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -582,25 +610,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,13 +640,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,37 +706,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,31 +748,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,7 +760,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,43 +784,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,6 +801,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -795,7 +832,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,17 +848,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -843,18 +869,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -873,151 +892,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1372,24 +1400,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:XFD24"/>
+  <dimension ref="A1:XFD23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.7" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.4266666666667" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.7133333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="51" style="2" customWidth="1"/>
     <col min="4" max="4" width="27.5733333333333" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.8" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.14" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.8533333333333" style="2" customWidth="1"/>
     <col min="7" max="7" width="10.7133333333333" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.14" style="2" customWidth="1"/>
     <col min="9" max="9" width="9" style="2"/>
@@ -50643,7 +50671,7 @@
       <c r="XFC4" s="8"/>
       <c r="XFD4" s="8"/>
     </row>
-    <row r="5" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="5" customHeight="1" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -50666,7 +50694,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="6" customHeight="1" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -50677,299 +50705,315 @@
         <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="7" customHeight="1" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="8" customHeight="1" spans="1:7">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="9" customHeight="1" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="10" customHeight="1" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="11" customHeight="1" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>45</v>
+      <c r="C11" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="12" customHeight="1" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
+      <c r="B12" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="13" customHeight="1" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>50</v>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="14" customHeight="1" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="15" s="2" customFormat="1" customHeight="1" spans="1:10">
+    <row r="15" customHeight="1" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="16" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="16" customHeight="1" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J16" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="17" s="2" customFormat="1" customHeight="1" spans="1:10">
+    <row r="17" customHeight="1" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
-    <row r="18" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="18" customHeight="1" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="19" customHeight="1" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="20" customHeight="1" spans="1:10">
       <c r="A20" s="2" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>69</v>
+        <v>76</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J20" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="21" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="21" customHeight="1" spans="1:10">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>36</v>
+        <v>81</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J21" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="22" s="2" customFormat="1" customHeight="1" spans="1:7">
+    <row r="22" customHeight="1" spans="1:10">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="J22" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="23" s="2" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>75</v>
+    <row r="23" s="7" customFormat="1" ht="15" customHeight="1" spans="1:19">
+      <c r="A23" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>77</v>
+      <c r="C23" s="2" t="s">
+        <v>86</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" s="7" customFormat="1" ht="15" customHeight="1" spans="1:19">
-      <c r="A24" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50984,22 +51028,22 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.6" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.2" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.85333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5.57333333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.14" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -51016,266 +51060,266 @@
     </row>
     <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2">
         <v>2</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B23" s="2">
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -51296,31 +51340,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-    <col min="2" max="2" width="9.3" customWidth="1"/>
-    <col min="3" max="3" width="28.7" customWidth="1"/>
+    <col min="1" max="1" width="9.42666666666667" customWidth="1"/>
+    <col min="2" max="2" width="9.28666666666667" customWidth="1"/>
+    <col min="3" max="3" width="28.7133333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>